<commit_message>
Excluded data after screening for very low quality responses, and likely AI responses.
</commit_message>
<xml_diff>
--- a/UI-Eval-Survey-Data/results/flagged_participants_summary.xlsx
+++ b/UI-Eval-Survey-Data/results/flagged_participants_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hgs52/Documents/Github/AI-UI-Ethics-Evaluations/UI-Eval-Survey-Data/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95B4BA9-41B3-7745-90F1-18920251D477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9D1E68-1EFA-684C-849B-473E70126A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="37360" windowHeight="20980" activeTab="2" xr2:uid="{FF812AA5-02D0-AE4B-9D6E-6A121C957A9F}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="37360" windowHeight="20980" activeTab="1" xr2:uid="{FF812AA5-02D0-AE4B-9D6E-6A121C957A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="flagged_participants_summar " sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="151">
   <si>
     <t>PROLIFIC_PID</t>
   </si>
@@ -472,6 +472,27 @@
   </si>
   <si>
     <t>F:UEQ</t>
+  </si>
+  <si>
+    <t>Low effort but still fine</t>
+  </si>
+  <si>
+    <t>Good response</t>
+  </si>
+  <si>
+    <t>Good Response</t>
+  </si>
+  <si>
+    <t>Low quality</t>
+  </si>
+  <si>
+    <t>Sus in a different way</t>
+  </si>
+  <si>
+    <t>Low Quality</t>
+  </si>
+  <si>
+    <t>Short but acceptable</t>
   </si>
 </sst>
 </file>
@@ -1464,8 +1485,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5512,19 +5533,19 @@
         <v>10</v>
       </c>
       <c r="D99" s="3">
-        <v>3.315555555555556</v>
+        <v>3.31555555555556</v>
       </c>
       <c r="E99" s="3">
-        <v>4.2928395061111111</v>
+        <v>4.2928395061111102</v>
       </c>
       <c r="F99" s="3">
-        <v>50.888888888888886</v>
+        <v>50.8888888888889</v>
       </c>
       <c r="G99" s="3">
-        <v>149.91999999999996</v>
+        <v>149.91999999999999</v>
       </c>
       <c r="H99" s="3">
-        <v>4549.632098883555</v>
+        <v>4549.6320988835596</v>
       </c>
     </row>
   </sheetData>
@@ -5660,8 +5681,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5722,7 +5743,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -5763,7 +5784,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -5946,7 +5967,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -5989,7 +6010,7 @@
     </row>
     <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -6032,7 +6053,7 @@
     </row>
     <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -6117,7 +6138,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -6158,7 +6179,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -6199,7 +6220,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>95</v>
       </c>
@@ -6240,7 +6261,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -6281,7 +6302,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -6322,7 +6343,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -6415,7 +6436,7 @@
     </row>
     <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -6463,7 +6484,7 @@
     <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -6504,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -6544,7 +6565,7 @@
     </row>
     <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6582,7 +6603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -6620,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -6658,7 +6679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -6697,7 +6718,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -6735,7 +6756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -6874,7 +6895,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -6918,7 +6939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -6962,7 +6983,7 @@
     <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -7002,7 +7023,7 @@
     </row>
     <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -7046,7 +7067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -7090,7 +7111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -7129,7 +7150,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -7179,7 +7200,7 @@
     <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -7218,7 +7239,7 @@
       </c>
     </row>
     <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -7260,7 +7281,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -7301,7 +7322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -7342,7 +7363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>108</v>
       </c>
@@ -7388,7 +7409,7 @@
     <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>97</v>
       </c>
@@ -7429,7 +7450,7 @@
     <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>41</v>
       </c>
@@ -7473,7 +7494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>68</v>
       </c>
@@ -7513,7 +7534,7 @@
     </row>
     <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -7552,7 +7573,7 @@
       </c>
     </row>
     <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>96</v>
       </c>
@@ -7592,7 +7613,7 @@
     </row>
     <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -7660,7 +7681,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" s="3" t="s">
         <v>137</v>
       </c>
@@ -7677,7 +7698,7 @@
         <v>4.1877192981842093</v>
       </c>
       <c r="F97" s="4">
-        <f t="shared" si="0"/>
+        <f>AVERAGEIF($P$2:$P$95,"",F2:F95)</f>
         <v>53.94736842105263</v>
       </c>
       <c r="G97" s="4">
@@ -7689,7 +7710,7 @@
         <v>4798.7099416342098</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" s="2" t="s">
         <v>135</v>
       </c>
@@ -7712,7 +7733,7 @@
         <v>2408.0685940881222</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" s="3" t="s">
         <v>136</v>
       </c>
@@ -7761,6 +7782,11 @@
   </sheetData>
   <autoFilter ref="A1:P99" xr:uid="{9CBFAFF1-6610-3649-B6A1-C1113F478D26}">
     <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="15">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
@@ -7889,9 +7915,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L100" sqref="L100"/>
+      <selection pane="topRight" activeCell="A48" sqref="A32:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7955,7 +7981,7 @@
     <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -7992,9 +8018,12 @@
       <c r="L7" t="b">
         <v>0</v>
       </c>
+      <c r="O7" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -8031,8 +8060,11 @@
       <c r="L9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -8075,9 +8107,12 @@
       <c r="N10" t="b">
         <v>0</v>
       </c>
+      <c r="O10" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -8118,7 +8153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -8160,18 +8195,21 @@
       </c>
       <c r="N13" t="b">
         <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -8209,7 +8247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -8250,8 +8288,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -8292,7 +8330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -8335,8 +8373,11 @@
       <c r="N27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -8377,7 +8418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -8421,9 +8462,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -8460,8 +8501,14 @@
       <c r="L32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O32" t="s">
+        <v>147</v>
+      </c>
+      <c r="P32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -8562,7 +8609,7 @@
     <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -8608,7 +8655,7 @@
     </row>
     <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -8646,7 +8693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -8731,8 +8778,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -8770,7 +8817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -8808,12 +8855,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -8850,9 +8897,15 @@
       <c r="L55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N55" t="b">
+        <v>1</v>
+      </c>
+      <c r="O55" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -8890,7 +8943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -8934,7 +8987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -8972,8 +9025,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -9011,8 +9064,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -9053,10 +9106,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -9100,7 +9153,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>113</v>
       </c>
@@ -9147,7 +9200,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>94</v>
       </c>
@@ -9186,7 +9239,7 @@
       </c>
     </row>
     <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -9224,7 +9277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>50</v>
       </c>
@@ -9265,7 +9318,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>61</v>
       </c>
@@ -9311,7 +9364,7 @@
     </row>
     <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>102</v>
       </c>
@@ -9349,7 +9402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -9386,9 +9439,12 @@
       <c r="L77" t="b">
         <v>0</v>
       </c>
+      <c r="O77" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>25</v>
       </c>
@@ -9427,7 +9483,7 @@
       </c>
     </row>
     <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>29</v>
       </c>
@@ -9474,7 +9530,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>57</v>
       </c>
@@ -9513,7 +9569,7 @@
       </c>
     </row>
     <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -9551,7 +9607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -9589,7 +9645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>56</v>
       </c>
@@ -9633,7 +9689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -9677,7 +9733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -9724,7 +9780,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>81</v>
       </c>
@@ -9771,7 +9827,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>30</v>
       </c>
@@ -9818,7 +9874,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>21</v>
       </c>
@@ -9856,7 +9912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>83</v>
       </c>
@@ -9897,7 +9953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>71</v>
       </c>
@@ -9935,7 +9991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>112</v>
       </c>
@@ -9976,7 +10032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>86</v>
       </c>
@@ -10020,36 +10076,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" s="2" t="s">
         <v>143</v>
       </c>
       <c r="C96" s="2">
-        <f>AVERAGEIF($O$2:$O$95,"",C2:C95)</f>
+        <f>AVERAGEIF($P$2:$P$95,"",C2:C95)</f>
         <v>10</v>
       </c>
       <c r="D96" s="5">
-        <f t="shared" ref="D96:H96" si="0">AVERAGEIF($O$2:$O$95,"",D2:D95)</f>
-        <v>3.7450000000000001</v>
+        <f>AVERAGEIF($P$2:$P$95,"",D2:D95)</f>
+        <v>3.8717391304347823</v>
       </c>
       <c r="E96" s="5">
-        <f t="shared" si="0"/>
-        <v>5.1066666666499998</v>
+        <f t="shared" ref="E96:H96" si="0">AVERAGEIF($P$2:$P$95,"",E2:E95)</f>
+        <v>4.5770531400434775</v>
       </c>
       <c r="F96" s="5">
-        <f t="shared" si="0"/>
-        <v>46</v>
+        <f>AVERAGEIF($P$2:$P$95,"",F2:F95)</f>
+        <v>43.260869565217391</v>
       </c>
       <c r="G96" s="5">
         <f t="shared" si="0"/>
-        <v>98.751250000000027</v>
+        <v>83.498913043478268</v>
       </c>
       <c r="H96" s="5">
         <f t="shared" si="0"/>
-        <v>2637.1640277392498</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+        <v>2350.3950482895211</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="4"/>
@@ -10058,7 +10114,7 @@
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" s="2" t="s">
         <v>135</v>
       </c>
@@ -10066,22 +10122,27 @@
         <v>10</v>
       </c>
       <c r="D98" s="5">
+        <f>AVERAGE(D7:D95)</f>
         <v>3.8265306122448974</v>
       </c>
       <c r="E98" s="5">
+        <f t="shared" ref="E98:H98" si="1">AVERAGE(E7:E95)</f>
         <v>4.8868480725510199</v>
       </c>
       <c r="F98" s="5">
+        <f t="shared" si="1"/>
         <v>43.877551020408163</v>
       </c>
       <c r="G98" s="5">
+        <f t="shared" si="1"/>
         <v>92.968367346938834</v>
       </c>
       <c r="H98" s="5">
+        <f t="shared" si="1"/>
         <v>2408.0685940881222</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" s="3" t="s">
         <v>136</v>
       </c>
@@ -10107,6 +10168,11 @@
   </sheetData>
   <autoFilter ref="A1:P99" xr:uid="{9CBFAFF1-6610-3649-B6A1-C1113F478D26}">
     <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="15">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>

</xml_diff>